<commit_message>
update missing table to include racial disparity variables
</commit_message>
<xml_diff>
--- a/table2.xlsx
+++ b/table2.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -404,39 +404,34 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>unemploymentrate_2011</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0.09</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.07</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>&lt;0.001</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>unemploymentrate_2012</t>
+          <t>unemploymentrate_2011</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.082</t>
+          <t>0.09</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.066</t>
+          <t>0.07</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -448,39 +443,34 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>unemploymentrate_2013</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0.076</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.063</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>&lt;0.001</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>unemploymentrate_2014</t>
+          <t>unemploymentrate_2012</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>0.065</t>
+          <t>0.082</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.055</t>
+          <t>0.066</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -492,39 +482,34 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>uninsuredrate_2010</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>0.18</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.21</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>&lt;0.001</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>uninsuredrate_2011</t>
+          <t>unemploymentrate_2013</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>0.18</t>
+          <t>0.076</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.19</t>
+          <t>0.063</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -536,39 +521,34 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>uninsuredrate_2012</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>0.17</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.19</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>&lt;0.001</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>uninsuredrate_2013</t>
+          <t>unemploymentrate_2014</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>0.17</t>
+          <t>0.065</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.20</t>
+          <t>0.055</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -580,215 +560,190 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>uninsuredrate_2014</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>0.14</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.16</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>&lt;0.001</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>childpoverty_2010</t>
+          <t>uninsuredrate_2010</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>0.24</t>
+          <t>0.18</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.24</t>
+          <t>0.21</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.96</t>
+          <t>&lt;0.001</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>childpoverty_2011</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>0.25</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0.24</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>0.27</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>childpoverty_2012</t>
+          <t>uninsuredrate_2011</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>0.25</t>
+          <t>0.18</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>0.24</t>
+          <t>0.19</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.12</t>
+          <t>&lt;0.001</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>childpoverty_2013</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>0.25</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>0.24</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>0.077</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>childpoverty_2014</t>
+          <t>uninsuredrate_2012</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>0.24</t>
+          <t>0.17</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>0.23</t>
+          <t>0.19</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.055</t>
+          <t>&lt;0.001</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>YPLLRate_2015</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>7,947</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>8,210</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>0.074</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>YPLLRate_2019</t>
+          <t>uninsuredrate_2013</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>8,443</t>
+          <t>0.17</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>9,023</t>
+          <t>0.20</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.003</t>
+          <t>&lt;0.001</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>PCPRate_2010</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>41</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>&lt;0.001</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>PCPRate_2011</t>
+          <t>uninsuredrate_2014</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>0.14</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>0.16</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -800,391 +755,346 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>PCPRate_2012</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>0.001</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>PCPRate_2013</t>
+          <t>childpoverty_2010</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>0.24</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>0.24</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.007</t>
+          <t>0.96</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>PCPRate_2014</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>49</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>&lt;0.001</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>obesity_2010</t>
+          <t>childpoverty_2011</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>28.4</t>
+          <t>0.25</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>27.8</t>
+          <t>0.24</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>&lt;0.001</t>
+          <t>0.27</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>obesity_2011</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>29.1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>28.3</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>&lt;0.001</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>obesity_2012</t>
+          <t>childpoverty_2012</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>30.5</t>
+          <t>0.25</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>29.7</t>
+          <t>0.24</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>&lt;0.001</t>
+          <t>0.12</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>obesity_2013</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>30.5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>29.7</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>&lt;0.001</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>obesity_2014</t>
+          <t>childpoverty_2013</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>30.7</t>
+          <t>0.25</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>30.1</t>
+          <t>0.24</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>&lt;0.001</t>
+          <t>0.077</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>inactivity_2011</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>27.0</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>27.2</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>0.26</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>inactivity_2012</t>
+          <t>childpoverty_2014</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>27.7</t>
+          <t>0.24</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>28.5</t>
+          <t>0.23</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>&lt;0.001</t>
+          <t>0.055</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>inactivity_2013</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>27.7</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>28.5</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>&lt;0.001</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>inactivity_2014</t>
+          <t>YPLLRate_2015</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>27.7</t>
+          <t>7,947</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>28.6</t>
+          <t>8,210</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>&lt;0.001</t>
+          <t>0.074</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>somecollege_2010</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>&lt;0.001</t>
+          <t>149</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>somecollege_2011</t>
+          <t>YPLLRate_2019</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>8,443</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>9,023</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.057</t>
+          <t>0.003</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>somecollege_2012</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>0.10</t>
+          <t>234</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>somecollege_2013</t>
+          <t>PCPRate_2010</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>63</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>41</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.073</t>
+          <t>&lt;0.001</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>somecollege_2014</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>56</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>0.17</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>highschool_2010</t>
+          <t>PCPRate_2011</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>61</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>39</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1196,132 +1106,1031 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>highschool_2011</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>78</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>82</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>&lt;0.001</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>highschool_2012</t>
+          <t>PCPRate_2012</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>82</t>
+          <t>61</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>87</t>
+          <t>53</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>&lt;0.001</t>
+          <t>0.001</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>highschool_2013</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>82</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>86</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>&lt;0.001</t>
+          <t>181</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>highschool_2014</t>
+          <t>PCPRate_2013</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>82</t>
+          <t>56</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>50</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>0.26</t>
+          <t>0.007</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Population</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>122,645</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>23,990</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>&lt;0.001</t>
+          <t>128</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
+          <t>PCPRate_2014</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>&lt;0.001</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>144</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>obesity_2010</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>28.4</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>27.8</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>&lt;0.001</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>obesity_2011</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>29.1</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>28.3</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>&lt;0.001</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>obesity_2012</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>30.5</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>29.7</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>&lt;0.001</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>obesity_2013</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>30.5</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>29.7</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>&lt;0.001</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>obesity_2014</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>30.7</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>30.1</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>&lt;0.001</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>inactivity_2011</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>27.0</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>27.2</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>0.26</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>inactivity_2012</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>27.7</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>28.5</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>&lt;0.001</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>inactivity_2013</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>27.7</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>28.5</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>&lt;0.001</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>inactivity_2014</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>27.7</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>28.6</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>&lt;0.001</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>somecollege_2010</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>&lt;0.001</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>somecollege_2011</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>0.057</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>somecollege_2012</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>somecollege_2013</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>0.073</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>somecollege_2014</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>0.17</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>highschool_2010</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>&lt;0.001</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>highschool_2011</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>&lt;0.001</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>118</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>highschool_2012</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>87</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>&lt;0.001</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>highschool_2013</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>86</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>&lt;0.001</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>highschool_2014</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>0.26</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>456</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>blwt</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>0.015</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>170</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>hpnon</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>0.20</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Population</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>122,645</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>23,990</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>&lt;0.001</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
           <t>PopDensity</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="B90" t="inlineStr">
         <is>
           <t>97</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="C90" t="inlineStr">
         <is>
           <t>135</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="D90" t="inlineStr">
         <is>
           <t>0.50</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>

</xml_diff>